<commit_message>
files from lecture and practical
</commit_message>
<xml_diff>
--- a/ASSESSMENT/Coursework1_AnalysingModels/ABM 2022 - CW2 - Assessment Criteria.xlsx
+++ b/ASSESSMENT/Coursework1_AnalysingModels/ABM 2022 - CW2 - Assessment Criteria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tpe03/OneDrive - University College London/Teaching_MSc_MRes/ABM 2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/ucfnbsu_ucl_ac_uk/Documents/#CASA0011__AgentbasedModellingForSpatialSystems/CASA0011ABM/ASSESSMENT/Coursework1_AnalysingModels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{24BD8DC1-7FEF-AD4B-8D2B-4E556EE3419D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{24BD8DC1-7FEF-AD4B-8D2B-4E556EE3419D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{365EF619-2817-428D-8098-C667825677FA}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="27760" windowHeight="14880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,77 +44,82 @@
  (4 possible marks)</t>
   </si>
   <si>
+    <t>Interpretation and Analysis
+ (6 possible marks)</t>
+  </si>
+  <si>
+    <t>A clear and well-structured report. High quality writing.</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>An adequate report, though there may be significant issues of clarity, structure or quality of writing.</t>
+  </si>
+  <si>
+    <t>Serious issues of clarity, structure or quality of writing, such that the report is missing key information or is difficult to understand.</t>
+  </si>
+  <si>
+    <t>Results are communicated visually with accurate and clear figures.</t>
+  </si>
+  <si>
+    <t>An attempt has been made to communicate results visually, though there may be some issues of presentation or accuracy.</t>
+  </si>
+  <si>
+    <t>Visual communication of results is either not attempted or poorly executed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An attempt has been made to approach the task systematically, though it is not particularly comprehensive. There may be ambiguities in how the approach is communicated. </t>
+  </si>
+  <si>
+    <t>The task has been tackled systematically. The explanation of the approach may omit certain details or the range of scenarios considered could have been broader.</t>
+  </si>
+  <si>
+    <t>The task has not been approached systematically, or a systematic approach has been discussed, but not followed.</t>
+  </si>
+  <si>
+    <t>Results are interpreted and analysed to some extent, though there are weaknesses in understanding, either of the overall model, of statistical details, or of the metrics considered.</t>
+  </si>
+  <si>
+    <t>Results are interpreted and analysed clearly, though there are small issues of understanding or of balance between considering specific details and the big picture.</t>
+  </si>
+  <si>
+    <t>Analysis and interpretation is absent, unclear or incorrect.</t>
+  </si>
+  <si>
+    <t>CASA0011 - Agent-Based Modelling - Coursework 2 - SugarScape - Mark Scheme</t>
+  </si>
+  <si>
+    <t>A competent report, with only minor weaknesses of clarity, structure or quality of writing.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
     <t>Communication
  (4 possible marks)</t>
-  </si>
-  <si>
-    <t>Interpretation and Analysis
- (6 possible marks)</t>
-  </si>
-  <si>
-    <t>A clear and well-structured report. High quality writing.</t>
-  </si>
-  <si>
-    <t>0-1</t>
-  </si>
-  <si>
-    <t>A competent report, with only minor weaknesses of clarity, structure or quality of writing.</t>
-  </si>
-  <si>
-    <t>An adequate report, though there may be significant issues of clarity, structure or quality of writing.</t>
-  </si>
-  <si>
-    <t>Serious issues of clarity, structure or quality of writing, such that the report is missing key information or is difficult to understand.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>Results are communicated visually with highly appropriate, considered and elegant figures.</t>
-  </si>
-  <si>
-    <t>Results are communicated visually with accurate and clear figures.</t>
-  </si>
-  <si>
-    <t>An attempt has been made to communicate results visually, though there may be some issues of presentation or accuracy.</t>
-  </si>
-  <si>
-    <t>Visual communication of results is either not attempted or poorly executed.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Results are interpreted and analysed clearly, demonstrating an excellent understanding of the model and the metrics studied.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <t>The task has been tackled with a flawlessly systematic approach, explained with no ambiguity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An attempt has been made to approach the task systematically, though it is not particularly comprehensive. There may be ambiguities in how the approach is communicated. </t>
-  </si>
-  <si>
-    <t>The task has been tackled systematically. The explanation of the approach may omit certain details or the range of scenarios considered could have been broader.</t>
-  </si>
-  <si>
-    <t>The task has not been approached systematically, or a systematic approach has been discussed, but not followed.</t>
-  </si>
-  <si>
-    <t>Results are interpreted and analysed clearly, demonstrating an excellent understanding of the model and the metrics studied.</t>
-  </si>
-  <si>
-    <t>Results are interpreted and analysed to some extent, though there are weaknesses in understanding, either of the overall model, of statistical details, or of the metrics considered.</t>
-  </si>
-  <si>
-    <t>Results are interpreted and analysed clearly, though there are small issues of understanding or of balance between considering specific details and the big picture.</t>
-  </si>
-  <si>
-    <t>Analysis and interpretation is absent, unclear or incorrect.</t>
-  </si>
-  <si>
-    <t>CASA0011 - Agent-Based Modelling - Coursework 2 - SugarScape - Mark Scheme</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -152,7 +157,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -224,7 +229,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -505,22 +510,22 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.125" style="1" customWidth="1"/>
     <col min="2" max="5" width="25" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="5"/>
       <c r="B2" s="6">
         <v>4</v>
@@ -532,44 +537,44 @@
         <v>2</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="150" customHeight="1">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="150" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="10"/>
       <c r="B5" s="6">
         <v>6</v>
@@ -584,38 +589,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="150" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="150" customHeight="1">
+      <c r="A7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="E7" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>